<commit_message>
adding latest inter coder reliability allocation csv and the latest responses csv
</commit_message>
<xml_diff>
--- a/inter-coder-reliability-data.xlsx
+++ b/inter-coder-reliability-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23906"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23921"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_8f6\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D03B5E23-05DA-4EC8-8875-7F78FE78DAF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7BC75B9-F572-4171-B99A-2EB4483DCBCF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-40395" yWindow="2415" windowWidth="28800" windowHeight="23355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="462">
   <si>
     <t>ID</t>
   </si>
@@ -1483,6 +1483,320 @@
   </si>
   <si>
     <t>VIR - United States Virgin Islands</t>
+  </si>
+  <si>
+    <t>Israa Mohammed</t>
+  </si>
+  <si>
+    <t>israa.mohammed1@alumni.lshtm.ac.uk</t>
+  </si>
+  <si>
+    <t>As noted in the  Ministry of Health's website "As from Saturday 17th October 2020 it is mandatory to wear a face mask or visor outside residence both when going to an indoor place and outdoors."
+Sources:
+https://web.archive.org/web/20210311074716/https://deputyprimeminister.gov.mt/en/health-promotion/covid-19/Pages/frequently-asked-questions.aspx
+https://web.archive.org/web/20210311074837/https://www.mondaq.com/operational-impacts-and-strategy/997658/prevention-is-better-than-cure-malta-introduces-face-mask-requirement-at-all-times-and-in-all-places</t>
+  </si>
+  <si>
+    <t>Dan Grinevics</t>
+  </si>
+  <si>
+    <t>daniels.grinevics@sant.ox.ac.uk</t>
+  </si>
+  <si>
+    <t>Since 27 February 2021 and until 22 March (under Decree-Law no.46), masks are mandatory in all public spaces both outdoors and indoors except where a person is alone or together with the cohabitant nucleus. Coding this as 3G because it refers to all public spaces and situations when social distancing is not possible. 
+https://web.archive.org/web/20201202210103/https://www.visitsanmarino.com/en/visitnews/Informazioni-utili-COVID-19.html</t>
+  </si>
+  <si>
+    <t>According to the U.S. embassy in Somalia, public transportation is operating. There was no indication that masks are required or that there are capacity restrictions.
+source: https://archive.ph/Yv2fN</t>
+  </si>
+  <si>
+    <t>I found many articles that state the vaccine is available and is free for elderly and vulnerable population.
+-------
+https://web.archive.org/web/20210314153123/https://abcnews.go.com/International/wireStory/algeria-launches-covid-19-vaccination-campaign-75578956
+https://web.archive.org/web/20210314153424/https://www.usnews.com/news/health-news/articles/2021-01-30/algeria-starts-covid-19-vaccination-drive-with-russian-shots
+https://web.archive.org/web/20210214195206/https://www.reuters.com/article/us-health-coronavirus-algeria-russia-idUSKBN2A11L6
+https://web.archive.org/web/20210314154358/https://www.peacefmonline.com/pages/local/news/202012/433991.php
+https://web.archive.org/web/20210314154508/https://nehandaradio.com/2020/12/04/algeria-to-offer-free-covid-vaccine-from-next-month/</t>
+  </si>
+  <si>
+    <t>DZA - Algeria</t>
+  </si>
+  <si>
+    <t>Commercial establishments will be open from 9 a.m. – 7 p.m. Monday – Saturday, and 9 a.m. – 4 p.m. on Sunday. Restaurants may remain open until 8 p.m. every day.  Public and private sector establishments will be held responsible for non-compliance with safety measures.
+https://web.archive.org/save/https://mz.usembassy.gov/covid-19-information/</t>
+  </si>
+  <si>
+    <t>Ursula Panzner</t>
+  </si>
+  <si>
+    <t>Ursula.Panzner1@student.lshtm.ac.uk</t>
+  </si>
+  <si>
+    <t>Note: no tracing; source: /web/20210315095951/https://ourworldindata.org/grapher/covid-contact-tracing?stackMode=absolute&amp;time=2021-03-14&amp;country=®ion=World</t>
+  </si>
+  <si>
+    <t>Nicole Gump</t>
+  </si>
+  <si>
+    <t>ngump@microsoft.com</t>
+  </si>
+  <si>
+    <t>Some autonomous communities have no limitation on movements between territories while others do:
+https://web.archive.org/web/20210120033448/https://www.mscbs.gob.es/en/profesionales/saludPublica/ccayes/alertasActual/nCov/estrategia/medidasPrevCCAA.htm</t>
+  </si>
+  <si>
+    <t>The first references shows public events such as "sports events" are being held, though they may have attendance caps.... the second reference indicates that "entertainment facilities" are open
+Published March 13, 2021: South Korea reported a three-week high of 488 new Covid-19 cases on Friday, prompting the authorities to extend social-distancing measures for two weeks, including a ban on gatherings of more than four people and attendance caps at schools, religious activities and sports events. The country’s total number of cases stands at 94,686, with 1,662 related deaths. https://web.archive.org/web/20210315230605/https://www.scmp.com/week-asia/politics/article/3125280/south-koreas-gyeonggi-province-mandatory-coronavirus-testing
+QR code-based access to facilities. Korea has a QR code-based registration system for patrons at restaurants, clubs, and other entertainment facilities across the country that are considered high risk for COVID-19.  This system enables the government to conduct contact tracing as COVID cases are identified. Information on this system and Korea’s “distancing in daily life” philosophy are available on the Ministry of Health and Welfare’s COVID-19 Portal. 
+https://web.archive.org/web/20210314162846/https://kr.usembassy.gov/022420-covid-19-information/</t>
+  </si>
+  <si>
+    <t>Chloeaxford@sky.com</t>
+  </si>
+  <si>
+    <t>No evidence of stay at home/ curfew restrictions in place specific to COVID-19. 
+https://web.archive.org/web/20210316102348/https://www.liberianobserver.com/?s=Liberia</t>
+  </si>
+  <si>
+    <t>LBR - Liberia</t>
+  </si>
+  <si>
+    <t>From March 13, the Almaty city administration closed cinemas and theatres. Trade centers are not allowed to operate during weekends.  On March 15, the Chief Sanitary Doctor of Nur-Sultan signed a new Decree for the following quarantine restrictions in the city starting from 00:00 of 18 March 2021. Operation of shopping/trade and entertainment centers houses will be banned on Sunday (allowed from Mon. to Sat. at a regular time). The work of cinemas will be suspended from March 18 in Nur-Sultan. Operation of fitness/spa/sports/saunas and recreation facilities will be prohibited on weekends, except for facilities participating in the Ashyq pilot project. Restaurants, cafes, bars, canteens will work from 07:00 to 22:00 throughout the week. The Decree has a provision on the transition to a remote form of work for at least 80 % of employees of all organizations, enterprises, regardless of the form of ownership and the full-time number of employees. Links: https://archive.ph/ipUV6 https://archive.ph/bfLES https://archive.ph/wmb0U</t>
+  </si>
+  <si>
+    <t>KAZ - Kazakhstan</t>
+  </si>
+  <si>
+    <t>From March 13, the Almaty city administration closed cinemas and theatres. Trade centers are not allowed to operate during weekends.  
+On March 15, the Chief Sanitary Doctor of Nur-Sultan signed a new Decree for the following quarantine restrictions in the city starting from 00:00 of 18 March 2021. 
+Operation of shopping/trade and entertainment centers houses will be banned on Sunday (allowed from Mon. to Sat. at a regular time). The work of cinemas will be suspended from March 18 in Nur-Sultan. Operation of fitness/spa/sports/saunas and recreation facilities will be prohibited on weekends, except for facilities participating in the Ashyq pilot project. Restaurants, cafes, bars, canteens will work from 07:00 to 22:00 throughout the week. The Decree has a provision on the transition to a remote form of work for at least 80 % of employees of all organizations, enterprises, regardless of the form of ownership and the full-time number of employees. Links: https://archive.ph/ipUV6 https://archive.ph/bfLES https://archive.ph/wmb0U</t>
+  </si>
+  <si>
+    <t>Tiwalade Ighomuaye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">According to the Netherlands Government's website, the rules up until March 15 have been extended till March 30th. 
+These are the restrictions till March 15th;
+Only go outside with members of your household, on your own or with 1 other person.
+The exception is;  
+Funerals may be attended by no more than 50 people.
+Most locations are closed, including:
+shops (except those selling essentials like foods). From 10 February all shops can offer a ‘click and collect service’. From 3 March shopping by appointment is permitted.
+theatres, concert halls, cinemas, casinos, etc.
+zoos, amusement parks, etc.
+indoor sports facilities such as gyms, swimming pools, saunas and spas.
+restaurants, bars and cafes.
+Please see: https://web.archive.org/web/20210318033958/https://www.government.nl/topics/coronavirus-covid-19/tackling-new-coronavirus-in-the-netherlands/coronavirus-measures-in-brief
+For the extension announcement please see: https://web.archive.org/web/20210318034129/https://www.government.nl/topics/coronavirus-covid-19/news/2021/03/08/further-easing-of-restrictions-not-yet-possible
+The following relevant modifications were made going forward from March 16;
+Shopping by appointment
+Shops will be allowed to admit 2 customers per floor or 1 customer per 25 square metres, up to a maximum of 50 customers at a time, if the shop is big enough. Everyone must stay 1.5 metres apart. The rule that appointments must be made at least 4 hours in advance still applies and each customer slot must be a minimum of 10 minutes.
+Sport
+Adults aged 27 and over can participate in sports activities at outdoor sports facilities in groups of up to 4 people. They must stay 1.5 metres apart. Adults aged 18 to 26 were already allowed to participate in team sports at sports facilities without staying 1.5 metres apart. The municipality may in certain cases also offer other opportunities for participating in organised sports.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLD - Netherlands </t>
+  </si>
+  <si>
+    <t>There is no evidence of public events held, curfews are in place, and large gatherings are also otherwise restricted.
+https://web.archive.org/web/20210320164340/https://jis.gov.jm/health-minister-reiterates-appeal-for-persons-to-obey-covid-19-protocols/
+https://web.archive.org/web/20210320162220/https://jm.usembassy.gov/covid-19-information-jamaica/
+https://web.archive.org/web/20210320164749/https://jis.gov.jm/media/2020/12/Disaster-Risk-Management-Enforcement-Measures-No.-16-Order.pdf</t>
+  </si>
+  <si>
+    <t>Jorge Luis Revilla</t>
+  </si>
+  <si>
+    <t>jl.revilla@microsoft.com</t>
+  </si>
+  <si>
+    <t>Argentina is offering an emergency bonus to formal workers, but the amount is half the minimum salary
+https://web.archive.org/web/20210123233054/https://www.argentina.gob.ar/economia/medidas-economicas-COVID19/ingresofamiliardeemergencia</t>
+  </si>
+  <si>
+    <t>Ana Lucia Villagran</t>
+  </si>
+  <si>
+    <t>alvillagranv@gmail.com</t>
+  </si>
+  <si>
+    <t>There are no curfews in place or stay at home requirements, but as part of the "Five Golden Rules" of COVID-19 prevention measures set by the Zambian Ministry of Health, staying at home is recommended. 
+"We must remain adherent to the public health guidance if we are to maintain the gains made in halting community transmission of Covid-19 as indicated by our reducing positivity rate. We must all play our part in ensuring adherence to the simple yet effective five golden rules. Remember to: 1) Mask up correctly and consistently; 2) Maintain physical distance; 3) Wash your hands frequently with soap and water or use hand sanitizer; 4) Avoid crowded places if possible, particularly super spreader events, or stay at home; and 5) Seek medical attention early if you are symptomatic.
+Have a safe and blessed Sunday.
+Hon. Dr. Jonas Chanda, MP.
+Minister of Health"
+Official information is kept most up-to-date on the ministry's official Facebook page (March 21 post): https://web.archive.org/web/20210321153609/https://www.facebook.com/login/?next=https%3A%2F%2Fwww.facebook.com%2Fmohzambia%2Fposts%2F1864231037084878%3F__tn__%3DK-R
+https://web.archive.org/web/20210321154438/https://zm.usembassy.gov/covid-19-information-2/</t>
+  </si>
+  <si>
+    <t>ZMB - Zambia</t>
+  </si>
+  <si>
+    <t>Victoria Cavero</t>
+  </si>
+  <si>
+    <t>victoriamcavero@gmail.com</t>
+  </si>
+  <si>
+    <t>1T</t>
+  </si>
+  <si>
+    <t>Public transport in some cities is open at a maximum of 50% of its capacity. 
+http://web.archive.org/web/20210319105503/https://www.elcomercio.com/actualidad/fronteras-cerradas-teletrabajo-control-aglomeraciones.html 
+http://web.archive.org/web/20210321213445/https://www.gov.uk/foreign-travel-advice/ecuador/coronavirus
+http://web.archive.org/web/20210318002522/https://ec.usembassy.gov/covid-19-information-ecu-2/</t>
+  </si>
+  <si>
+    <t>ECU - Ecuador</t>
+  </si>
+  <si>
+    <t>Ayanna Griffith</t>
+  </si>
+  <si>
+    <t>Ayanna.Griffith1@alumni.lshtm.ac.uk</t>
+  </si>
+  <si>
+    <t>Events are allowed to go ahead, but the government has issued hygiene restrictions, and recommendations on the number of individuals permitted to attend.
+"It is recommended to consider canceling indoor and outdoor events if they exceed the number of more than 100 or 500 respectively to minimize the impact of the epidemic over the economy and society. "
+Source: https://web.archive.org/web/20210322105619/https://covid19.mohw.gov.tw/en/cp-4786-53904-206.html
+This source was last updated on 16 March 2021. No further data has been found indicating that a different policy has been implemented.</t>
+  </si>
+  <si>
+    <t>TWN - Taiwan</t>
+  </si>
+  <si>
+    <t>There are some organization based websites, but I'm not seeing an official government website, presenting all the relevant Covid-19 information.</t>
+  </si>
+  <si>
+    <t>Charles Piñon</t>
+  </si>
+  <si>
+    <t>c.pinon@hotmail.com</t>
+  </si>
+  <si>
+    <t>Paraguay carries out a broad public information campaign either on traditional media and online through the Public Health and Social Welfare Ministry. Social media broadcasts have also been observed.
+https://web.archive.org/web/20210322200105/https://www.mspbs.gov.py/covid-19.php</t>
+  </si>
+  <si>
+    <t>Beginning March 8th, beaches can remain open until 5 p.m. on weekends and holidays. 
+Restaurants can seat up to 75 percent of their approved seating capacity, and they can seat more than six people at the same table if they are all in the same party.
+Masking requirements and social distancing remain in effect.
+http://web.archive.org/web/20210322221922/https://www.vi.gov/covid/news-post/governor-bryan-eases-some-covid-19-restrictions-for-restaurants-taxicabs-and-beaches/</t>
+  </si>
+  <si>
+    <t>Melissa Toh</t>
+  </si>
+  <si>
+    <t>meltoh.ps@icloud.com</t>
+  </si>
+  <si>
+    <t>Public events are banned, with private gatherings such as weddings, funerals and religious gatherings exempt.
+_______________________________________________
+Quote from article 1:
+" All public events and gatherings, including political events, are banned. Funerals, burials, and weddings are exempt but must not exceed 150 attendees. Bars, restaurants, and other establishments are open to the public but must close at 2100 nightly."
+Archived link 1:
+http://archive.today/2021.03.23-035141/https://www.garda.com/crisis24/news-alerts/445106/kenya-covid-19-restrictions-remain-largely-unchanged-feb-18-as-compared-with-those-in-force-in-late-january-update-18
+_______________________________________________
+Quote from article 2:
+"Places of worship may begin phased re-opening in conformity with applicable guidelines developed by the Inter-Faith Council.  The permitted maximum size of religious gatherings is increased to one third (1/3) of its normal sitting capacity.  The maximum number of persons permitted to attend funerals and weddings is reviewed upwards to 200, with all in attendance abiding with Ministry of Health Protocols."
+Archived link 2:
+http://archive.today/2021.03.23-035302/https://ke.usembassy.gov/covid-19-information/
+________________________________________________</t>
+  </si>
+  <si>
+    <t>KEN - Kenya</t>
+  </si>
+  <si>
+    <t>Private sector employees in Saudi Arabia can go back offices with minimal staff and strict following of coronavirus precautionary measures, the Ministry of Human Resources and Social Development announced on Wednesday.
+“The private sector can start working while following the precautionary and preventive measures announced by the ministry of health and supervising authorities,” the ministry said.
+The move is the latest of the Kingdom's announcements to ease the coronavirus restrictions, which saw the Kingdom under full lockdown at times, including during the Islamic celebration of Eid al-Fitr.
+https://web.archive.org/web/20210324093030/https://english.alarabiya.net/coronavirus/2020/05/27/Coronavirus-Private-sector-in-Saudi-Arabia-can-return-to-offices</t>
+  </si>
+  <si>
+    <t>Ayan Habane</t>
+  </si>
+  <si>
+    <t>ayanhabane@hotmail.co.uk</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anyone who has COVID symptoms, or has been in contact with those who have tested positive, or has been alerted via the Smittestopp-app must test for COVID (including children), countrywide. However, testing is organised differently in different municipalities. 
+https://web.archive.org/web/20210324125041/https://www.helsenorge.no/en/coronavirus/testing-symptoms-and-close-contacts/
+</t>
+  </si>
+  <si>
+    <t>NOR - Norway</t>
+  </si>
+  <si>
+    <t>Dagny Ahrend</t>
+  </si>
+  <si>
+    <t>dahrend01@qub.ac.uk</t>
+  </si>
+  <si>
+    <t>PCR and/or antigen tests are available at both private and government laboratories. Testing capacity has also been extended to rural health facilities.
+Link: https://web.archive.org/web/20210322163617/https://zw.usembassy.gov/covid-19-information-2/
+https://web.archive.org/web/20210324121540/https://reliefweb.int/report/zimbabwe/capacitating-rural-health-facilities-rapid-covid-19-testing</t>
+  </si>
+  <si>
+    <t>Farah Sayad</t>
+  </si>
+  <si>
+    <t>fsayad96@gmail.com</t>
+  </si>
+  <si>
+    <t>On 22 February, Saudi Arabia's Minister of Education announced that schools would continue with e-learning (distance education) "till the end of the current academic year." 
+https://archive.vn/mKigO 
+https://archive.vn/xB7fJ
+"Around 6 million students in different education stages in the kingdom have been taught online instead of attending classes as a precaution to limit the spread of the coronavirus."
+https://archive.vn/lT27a</t>
+  </si>
+  <si>
+    <t>Sharon Farrell</t>
+  </si>
+  <si>
+    <t>sharontheresefarrell@gmail.com</t>
+  </si>
+  <si>
+    <t>A report from February 2021 is the most recent policy update available on the Zambian government departments. It cites poor adherence to masking policy by the public and law enforcement. The second link shows the type of PPE required in different circumstances, but neither of these links offers a metric by which these "recommended" guidelines are enforced. Moreover, these guidelines are implemented across the state. Therefore, I gave the code 1G to H6 in Zambia.
+https://web.archive.org/web/20210328132715/http://www.parliament.gov.zm/sites/default/files/images/publication_docs/Ministerial%20Statement%20on%20the%20Status%20of%20COVID-19%20Situation%20in%20the%20Country..pdf 
+https://web.archive.org/web/20210328133417/https://www.moh.gov.zm/?wpfb_dl=147</t>
+  </si>
+  <si>
+    <t>Ziya Utku Karadeniz</t>
+  </si>
+  <si>
+    <t>ziya.karadeniz@boun.edu.tr</t>
+  </si>
+  <si>
+    <t>According to the Taoiseach Micheál Martin, the level 5 restrictions will continue until 5 April 2021. In level 5 restrictions, up to 6 people can attend a wedding and up to 10 can attend funerals. There is no allowance for the organized indoor, outdoor, exercise group activities, or sporting fixtures. All cultural attractions like museums, galleries are closed. Except for professional elite sports, horse-racing, and greyhound racing which took place behind closed doors, any training or matches are also not allowed. 
+https://web.archive.org/web/20210228085318/https://www.rte.ie/news/coronavirus/2021/0223/1198716-living-with-covid/
+https://web.archive.org/web/20210322051757/https://www.citizensinformation.ie/en/covid19/living_with_covid19_plan.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since, the info in the article says that gatherings are discouraged but there is no mention of restrictions in place or made mandatory, we will code it with 0.
+https://web.archive.org/web/20210329223917/https://blog.wego.com/solomon-islands-travel-restrictions-and-quarantine-requirements/
+</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/20210329224733/https://crisis24.garda.com/insights-intelligence/intelligence/risk-alerts/wip10011895117/bhutan-authorities-maintaining-nationwide-covid-19-measures-as-of-dec-14-update-16</t>
+  </si>
+  <si>
+    <t>Ehsan Rafian</t>
+  </si>
+  <si>
+    <t>On 21 March, Maduro announced two weeks of "radical quarantine" in Venezuela, which includes a set of restrictive measures to tighten the national quarantine. These enhanced restrictions began on 22 March and will continue until 4 April. 
+Maduro cited the recommendations of the presidential commission in charge of monitoring the coronavirus: "Minimize unnecessary population mobility, avoid concentrations of people in public spaces, reduce non-essential banking and commercial activities."
+https://web.archive.org/web/20210330201827/https://www.elnacional.com/venezuela/regimen-de-maduro-decreto-15-dias-de-cuarentena-radical-por-aumento-de-casos-de-covid-19/
+https://web.archive.org/web/20210330210759/https://twitter.com/NicolasMaduro/status/1374035170181971981
+https://archive.vn/DNwTH</t>
+  </si>
+  <si>
+    <t>VEN - Venezuela</t>
   </si>
   <si>
     <t>G96VzPWXk0-0uv5ouFLPkVSWvw_jDgZKm4LZGz53kfBUNUVEUzNPMElMVFcxSUNGNzFDOUZRSUxHQiQlQCN0PWcu</t>
@@ -1615,8 +1929,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:Q107" totalsRowShown="0">
-  <autoFilter ref="A1:Q107" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:Q137" totalsRowShown="0">
+  <autoFilter ref="A1:Q137" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="16"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Start time" dataDxfId="15"/>
@@ -1937,7 +2251,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R107"/>
+  <dimension ref="A1:R137"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
       <selection activeCell="Q4" sqref="Q4"/>
@@ -6627,6 +6941,1296 @@
       </c>
       <c r="P107" s="3"/>
       <c r="Q107" s="3"/>
+    </row>
+    <row r="108" spans="1:17" ht="165">
+      <c r="A108" s="2">
+        <v>109</v>
+      </c>
+      <c r="B108" s="1">
+        <v>44266.30878472222</v>
+      </c>
+      <c r="C108" s="1">
+        <v>44266.330208333333</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="H108" s="3"/>
+      <c r="I108" s="3"/>
+      <c r="J108" s="4">
+        <v>44266</v>
+      </c>
+      <c r="K108" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="L108" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="M108" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N108" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="O108" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P108" s="3"/>
+      <c r="Q108" s="3"/>
+    </row>
+    <row r="109" spans="1:17" ht="90">
+      <c r="A109" s="2">
+        <v>110</v>
+      </c>
+      <c r="B109" s="1">
+        <v>44266.826944444445</v>
+      </c>
+      <c r="C109" s="1">
+        <v>44266.84915509259</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="H109" s="3"/>
+      <c r="I109" s="3"/>
+      <c r="J109" s="4">
+        <v>44266</v>
+      </c>
+      <c r="K109" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="L109" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="M109" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N109" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="O109" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="P109" s="3"/>
+      <c r="Q109" s="3"/>
+    </row>
+    <row r="110" spans="1:17" ht="45">
+      <c r="A110" s="2">
+        <v>111</v>
+      </c>
+      <c r="B110" s="1">
+        <v>44268.713206018518</v>
+      </c>
+      <c r="C110" s="1">
+        <v>44268.722349537034</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="H110" s="3"/>
+      <c r="I110" s="3"/>
+      <c r="J110" s="4">
+        <v>44266</v>
+      </c>
+      <c r="K110" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L110" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="M110" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N110" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="O110" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="P110" s="3"/>
+      <c r="Q110" s="3"/>
+    </row>
+    <row r="111" spans="1:17" ht="150">
+      <c r="A111" s="2">
+        <v>112</v>
+      </c>
+      <c r="B111" s="1">
+        <v>44269.643252314818</v>
+      </c>
+      <c r="C111" s="1">
+        <v>44269.65828703704</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E111" s="2"/>
+      <c r="F111" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G111" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="H111" s="3"/>
+      <c r="I111" s="3"/>
+      <c r="J111" s="4">
+        <v>44269</v>
+      </c>
+      <c r="K111" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L111" s="8" t="s">
+        <v>391</v>
+      </c>
+      <c r="M111" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N111" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O111" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="P111" s="3"/>
+      <c r="Q111" s="3"/>
+    </row>
+    <row r="112" spans="1:17" ht="75">
+      <c r="A112" s="2">
+        <v>113</v>
+      </c>
+      <c r="B112" s="1">
+        <v>44269.718090277776</v>
+      </c>
+      <c r="C112" s="1">
+        <v>44269.722858796296</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E112" s="2"/>
+      <c r="F112" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G112" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="H112" s="3"/>
+      <c r="I112" s="3"/>
+      <c r="J112" s="4">
+        <v>44269</v>
+      </c>
+      <c r="K112" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L112" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="M112" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N112" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="O112" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="P112" s="3"/>
+      <c r="Q112" s="3"/>
+    </row>
+    <row r="113" spans="1:17" ht="45">
+      <c r="A113" s="2">
+        <v>114</v>
+      </c>
+      <c r="B113" s="1">
+        <v>44270.411006944443</v>
+      </c>
+      <c r="C113" s="1">
+        <v>44270.417060185187</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="G113" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="H113" s="3"/>
+      <c r="I113" s="3"/>
+      <c r="J113" s="4">
+        <v>44269</v>
+      </c>
+      <c r="K113" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L113" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="M113" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N113" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O113" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="P113" s="3"/>
+      <c r="Q113" s="3"/>
+    </row>
+    <row r="114" spans="1:17" ht="75">
+      <c r="A114" s="2">
+        <v>115</v>
+      </c>
+      <c r="B114" s="1">
+        <v>44270.600243055553</v>
+      </c>
+      <c r="C114" s="1">
+        <v>44270.616990740738</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E114" s="2"/>
+      <c r="F114" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G114" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="H114" s="3"/>
+      <c r="I114" s="3"/>
+      <c r="J114" s="4">
+        <v>44270</v>
+      </c>
+      <c r="K114" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="L114" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="M114" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N114" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O114" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="P114" s="3"/>
+      <c r="Q114" s="3"/>
+    </row>
+    <row r="115" spans="1:17" ht="255">
+      <c r="A115" s="2">
+        <v>116</v>
+      </c>
+      <c r="B115" s="1">
+        <v>44270.9528125</v>
+      </c>
+      <c r="C115" s="1">
+        <v>44270.965057870373</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E115" s="2"/>
+      <c r="F115" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="G115" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="H115" s="3"/>
+      <c r="I115" s="3"/>
+      <c r="J115" s="4">
+        <v>44270</v>
+      </c>
+      <c r="K115" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L115" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="M115" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N115" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="O115" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="P115" s="3"/>
+      <c r="Q115" s="3"/>
+    </row>
+    <row r="116" spans="1:17" ht="45">
+      <c r="A116" s="2">
+        <v>117</v>
+      </c>
+      <c r="B116" s="1">
+        <v>44271.404606481483</v>
+      </c>
+      <c r="C116" s="1">
+        <v>44271.433437500003</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="H116" s="3"/>
+      <c r="I116" s="3"/>
+      <c r="J116" s="4">
+        <v>44271</v>
+      </c>
+      <c r="K116" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L116" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="M116" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N116" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="O116" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="P116" s="3"/>
+      <c r="Q116" s="3"/>
+    </row>
+    <row r="117" spans="1:17" ht="135">
+      <c r="A117" s="2">
+        <v>118</v>
+      </c>
+      <c r="B117" s="1">
+        <v>44272.446921296294</v>
+      </c>
+      <c r="C117" s="1">
+        <v>44272.448472222219</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G117" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="H117" s="3"/>
+      <c r="I117" s="3"/>
+      <c r="J117" s="4">
+        <v>44272</v>
+      </c>
+      <c r="K117" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L117" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="M117" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N117" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="O117" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="P117" s="3"/>
+      <c r="Q117" s="3"/>
+    </row>
+    <row r="118" spans="1:17" ht="165">
+      <c r="A118" s="2">
+        <v>119</v>
+      </c>
+      <c r="B118" s="1">
+        <v>44272.448738425926</v>
+      </c>
+      <c r="C118" s="1">
+        <v>44272.449745370373</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="H118" s="3"/>
+      <c r="I118" s="3"/>
+      <c r="J118" s="4">
+        <v>44272</v>
+      </c>
+      <c r="K118" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="L118" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="M118" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N118" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="O118" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="P118" s="3"/>
+      <c r="Q118" s="3"/>
+    </row>
+    <row r="119" spans="1:17" ht="409.6">
+      <c r="A119" s="2">
+        <v>120</v>
+      </c>
+      <c r="B119" s="1">
+        <v>44273.11241898148</v>
+      </c>
+      <c r="C119" s="1">
+        <v>44273.157442129632</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="G119" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="H119" s="3"/>
+      <c r="I119" s="3"/>
+      <c r="J119" s="4">
+        <v>44272</v>
+      </c>
+      <c r="K119" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L119" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="M119" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N119" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="O119" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="P119" s="3"/>
+      <c r="Q119" s="3"/>
+    </row>
+    <row r="120" spans="1:17" ht="105">
+      <c r="A120" s="2">
+        <v>121</v>
+      </c>
+      <c r="B120" s="1">
+        <v>44275.678657407407</v>
+      </c>
+      <c r="C120" s="1">
+        <v>44275.701898148145</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E120" s="2"/>
+      <c r="F120" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H120" s="3"/>
+      <c r="I120" s="3"/>
+      <c r="J120" s="4">
+        <v>44275</v>
+      </c>
+      <c r="K120" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L120" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="M120" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N120" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="O120" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="P120" s="3"/>
+      <c r="Q120" s="3"/>
+    </row>
+    <row r="121" spans="1:17" ht="45">
+      <c r="A121" s="2">
+        <v>122</v>
+      </c>
+      <c r="B121" s="1">
+        <v>44276.193402777775</v>
+      </c>
+      <c r="C121" s="1">
+        <v>44276.198831018519</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E121" s="2"/>
+      <c r="F121" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="G121" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="H121" s="3"/>
+      <c r="I121" s="3"/>
+      <c r="J121" s="4">
+        <v>44275</v>
+      </c>
+      <c r="K121" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="L121" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="M121" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N121" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="O121" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P121" s="3"/>
+      <c r="Q121" s="3"/>
+    </row>
+    <row r="122" spans="1:17" ht="360">
+      <c r="A122" s="2">
+        <v>123</v>
+      </c>
+      <c r="B122" s="1">
+        <v>44276.634479166663</v>
+      </c>
+      <c r="C122" s="1">
+        <v>44276.660138888888</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E122" s="2"/>
+      <c r="F122" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="G122" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="H122" s="3"/>
+      <c r="I122" s="3"/>
+      <c r="J122" s="4">
+        <v>44276</v>
+      </c>
+      <c r="K122" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L122" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="M122" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N122" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="O122" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="P122" s="3"/>
+      <c r="Q122" s="3"/>
+    </row>
+    <row r="123" spans="1:17" ht="120">
+      <c r="A123" s="2">
+        <v>124</v>
+      </c>
+      <c r="B123" s="1">
+        <v>44276.758553240739</v>
+      </c>
+      <c r="C123" s="1">
+        <v>44276.900949074072</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E123" s="2"/>
+      <c r="F123" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="G123" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="H123" s="3"/>
+      <c r="I123" s="3"/>
+      <c r="J123" s="4">
+        <v>44276</v>
+      </c>
+      <c r="K123" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="L123" s="8" t="s">
+        <v>421</v>
+      </c>
+      <c r="M123" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N123" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="O123" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="P123" s="3"/>
+      <c r="Q123" s="3"/>
+    </row>
+    <row r="124" spans="1:17" ht="150">
+      <c r="A124" s="2">
+        <v>125</v>
+      </c>
+      <c r="B124" s="1">
+        <v>44277.447268518517</v>
+      </c>
+      <c r="C124" s="1">
+        <v>44277.461967592593</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E124" s="2"/>
+      <c r="F124" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="G124" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="H124" s="3"/>
+      <c r="I124" s="3"/>
+      <c r="J124" s="4">
+        <v>44277</v>
+      </c>
+      <c r="K124" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L124" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="M124" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N124" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="O124" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="P124" s="3"/>
+      <c r="Q124" s="3"/>
+    </row>
+    <row r="125" spans="1:17" ht="30">
+      <c r="A125" s="2">
+        <v>126</v>
+      </c>
+      <c r="B125" s="1">
+        <v>44277.65351851852</v>
+      </c>
+      <c r="C125" s="1">
+        <v>44277.658252314817</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E125" s="2"/>
+      <c r="F125" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="G125" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H125" s="3"/>
+      <c r="I125" s="3"/>
+      <c r="J125" s="4">
+        <v>44277</v>
+      </c>
+      <c r="K125" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L125" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="M125" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N125" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O125" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="P125" s="3"/>
+      <c r="Q125" s="3"/>
+    </row>
+    <row r="126" spans="1:17" ht="60">
+      <c r="A126" s="2">
+        <v>127</v>
+      </c>
+      <c r="B126" s="1">
+        <v>44277.826157407406</v>
+      </c>
+      <c r="C126" s="1">
+        <v>44277.848773148151</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E126" s="2"/>
+      <c r="F126" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="G126" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="H126" s="3"/>
+      <c r="I126" s="3"/>
+      <c r="J126" s="4">
+        <v>44277</v>
+      </c>
+      <c r="K126" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L126" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="M126" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N126" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O126" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="P126" s="3"/>
+      <c r="Q126" s="3"/>
+    </row>
+    <row r="127" spans="1:17" ht="90">
+      <c r="A127" s="2">
+        <v>128</v>
+      </c>
+      <c r="B127" s="1">
+        <v>44277.921400462961</v>
+      </c>
+      <c r="C127" s="1">
+        <v>44277.930590277778</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E127" s="2"/>
+      <c r="F127" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G127" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="H127" s="3"/>
+      <c r="I127" s="3"/>
+      <c r="J127" s="4">
+        <v>44277</v>
+      </c>
+      <c r="K127" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L127" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="M127" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N127" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="O127" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="P127" s="3"/>
+      <c r="Q127" s="3"/>
+    </row>
+    <row r="128" spans="1:17" ht="409.6">
+      <c r="A128" s="2">
+        <v>129</v>
+      </c>
+      <c r="B128" s="1">
+        <v>44278.159560185188</v>
+      </c>
+      <c r="C128" s="1">
+        <v>44278.167349537034</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E128" s="2"/>
+      <c r="F128" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="H128" s="3"/>
+      <c r="I128" s="3"/>
+      <c r="J128" s="4">
+        <v>44278</v>
+      </c>
+      <c r="K128" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L128" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="M128" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N128" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="O128" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="P128" s="3"/>
+      <c r="Q128" s="3"/>
+    </row>
+    <row r="129" spans="1:17" ht="150">
+      <c r="A129" s="2">
+        <v>130</v>
+      </c>
+      <c r="B129" s="1">
+        <v>44279.371388888889</v>
+      </c>
+      <c r="C129" s="1">
+        <v>44279.396585648145</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E129" s="2"/>
+      <c r="F129" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="G129" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="H129" s="3"/>
+      <c r="I129" s="3"/>
+      <c r="J129" s="4">
+        <v>44279</v>
+      </c>
+      <c r="K129" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L129" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="M129" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N129" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="O129" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="P129" s="3"/>
+      <c r="Q129" s="3"/>
+    </row>
+    <row r="130" spans="1:17" ht="120">
+      <c r="A130" s="2">
+        <v>131</v>
+      </c>
+      <c r="B130" s="1">
+        <v>44279.530289351853</v>
+      </c>
+      <c r="C130" s="1">
+        <v>44279.550578703704</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E130" s="2"/>
+      <c r="F130" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="G130" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="H130" s="3"/>
+      <c r="I130" s="3"/>
+      <c r="J130" s="4">
+        <v>44273</v>
+      </c>
+      <c r="K130" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="L130" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="M130" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N130" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="O130" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="P130" s="3"/>
+      <c r="Q130" s="3"/>
+    </row>
+    <row r="131" spans="1:17" ht="120">
+      <c r="A131" s="2">
+        <v>132</v>
+      </c>
+      <c r="B131" s="1">
+        <v>44279.475925925923</v>
+      </c>
+      <c r="C131" s="1">
+        <v>44279.642997685187</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E131" s="2"/>
+      <c r="F131" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="G131" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="H131" s="3"/>
+      <c r="I131" s="3"/>
+      <c r="J131" s="4">
+        <v>44279</v>
+      </c>
+      <c r="K131" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L131" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="M131" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N131" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="O131" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="P131" s="3"/>
+      <c r="Q131" s="3"/>
+    </row>
+    <row r="132" spans="1:17" ht="105">
+      <c r="A132" s="2">
+        <v>133</v>
+      </c>
+      <c r="B132" s="1">
+        <v>44283.498773148145</v>
+      </c>
+      <c r="C132" s="1">
+        <v>44283.516655092593</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E132" s="2"/>
+      <c r="F132" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="H132" s="3"/>
+      <c r="I132" s="3"/>
+      <c r="J132" s="4">
+        <v>44283</v>
+      </c>
+      <c r="K132" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="L132" s="8" t="s">
+        <v>447</v>
+      </c>
+      <c r="M132" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N132" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O132" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="P132" s="3"/>
+      <c r="Q132" s="3"/>
+    </row>
+    <row r="133" spans="1:17" ht="210">
+      <c r="A133" s="2">
+        <v>134</v>
+      </c>
+      <c r="B133" s="1">
+        <v>44283.563298611109</v>
+      </c>
+      <c r="C133" s="1">
+        <v>44283.566284722219</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E133" s="2"/>
+      <c r="F133" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="G133" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="H133" s="3"/>
+      <c r="I133" s="3"/>
+      <c r="J133" s="4">
+        <v>44283</v>
+      </c>
+      <c r="K133" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L133" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="M133" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N133" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="O133" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="P133" s="3"/>
+      <c r="Q133" s="3"/>
+    </row>
+    <row r="134" spans="1:17" ht="150">
+      <c r="A134" s="2">
+        <v>135</v>
+      </c>
+      <c r="B134" s="1">
+        <v>44284.541898148149</v>
+      </c>
+      <c r="C134" s="1">
+        <v>44284.554791666669</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E134" s="2"/>
+      <c r="F134" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="G134" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="H134" s="3"/>
+      <c r="I134" s="3"/>
+      <c r="J134" s="4">
+        <v>44250</v>
+      </c>
+      <c r="K134" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L134" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="M134" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N134" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="O134" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="P134" s="3"/>
+      <c r="Q134" s="3"/>
+    </row>
+    <row r="135" spans="1:17" ht="105">
+      <c r="A135" s="2">
+        <v>136</v>
+      </c>
+      <c r="B135" s="1">
+        <v>44284.942013888889</v>
+      </c>
+      <c r="C135" s="1">
+        <v>44284.94940972222</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E135" s="2"/>
+      <c r="F135" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G135" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="H135" s="3"/>
+      <c r="I135" s="3"/>
+      <c r="J135" s="4">
+        <v>44284</v>
+      </c>
+      <c r="K135" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L135" s="8" t="s">
+        <v>454</v>
+      </c>
+      <c r="M135" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N135" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O135" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="P135" s="3"/>
+      <c r="Q135" s="3"/>
+    </row>
+    <row r="136" spans="1:17" ht="30">
+      <c r="A136" s="2">
+        <v>137</v>
+      </c>
+      <c r="B136" s="1">
+        <v>44284.942488425928</v>
+      </c>
+      <c r="C136" s="1">
+        <v>44284.950069444443</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E136" s="2"/>
+      <c r="F136" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="G136" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="H136" s="3"/>
+      <c r="I136" s="3"/>
+      <c r="J136" s="4">
+        <v>44284</v>
+      </c>
+      <c r="K136" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="L136" s="8" t="s">
+        <v>455</v>
+      </c>
+      <c r="M136" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N136" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="O136" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="P136" s="3"/>
+      <c r="Q136" s="3"/>
+    </row>
+    <row r="137" spans="1:17" ht="285">
+      <c r="A137" s="2">
+        <v>138</v>
+      </c>
+      <c r="B137" s="1">
+        <v>44285.783518518518</v>
+      </c>
+      <c r="C137" s="1">
+        <v>44285.89135416667</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E137" s="2"/>
+      <c r="F137" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="G137" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="H137" s="3"/>
+      <c r="I137" s="3"/>
+      <c r="J137" s="4">
+        <v>44285</v>
+      </c>
+      <c r="K137" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L137" s="8" t="s">
+        <v>457</v>
+      </c>
+      <c r="M137" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N137" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O137" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="P137" s="3"/>
+      <c r="Q137" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6649,17 +8253,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>384</v>
+        <v>459</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>385</v>
+        <v>460</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>386</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -6669,6 +8273,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -6677,7 +8287,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001232BEEEE9047E4490583C45709DDAE2" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6fbf2cb7b50ab12ba1e89a3efb3d0ef9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a4433e03-c22d-4073-880d-28cc6965813d" xmlns:ns3="e6b6c2dd-0746-463e-a2fc-74accf0bcec0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c980077645cb3db6e195d37801db0483" ns2:_="" ns3:_="">
     <xsd:import namespace="a4433e03-c22d-4073-880d-28cc6965813d"/>
@@ -6888,20 +8498,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6381576-0096-40C2-841F-926831843C91}"/>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EDA661D-DF29-49D3-A0BD-A35617753F39}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D325DDFC-8A22-4969-BBED-5037ACC47378}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6381576-0096-40C2-841F-926831843C91}"/>
 </file>
</xml_diff>

<commit_message>
modify US allocation to pull 27 April sheet. Date collection mech still not fixed. Add latest results sheet. Add latest allocation CSV.
</commit_message>
<xml_diff>
--- a/inter-coder-reliability-data.xlsx
+++ b/inter-coder-reliability-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_8f6\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7BC75B9-F572-4171-B99A-2EB4483DCBCF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A32AC7AD-B235-4D42-989B-4F3FA9137481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-40395" yWindow="2415" windowWidth="28800" windowHeight="23355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="542">
   <si>
     <t>ID</t>
   </si>
@@ -1797,6 +1797,348 @@
   </si>
   <si>
     <t>VEN - Venezuela</t>
+  </si>
+  <si>
+    <t>Simon Powell</t>
+  </si>
+  <si>
+    <t>simonpo@microsoft.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The US Embassy reports that there are no restrictions on intercity or interstate travel - https://web.archive.org/web/20210331132431/https://ba.usembassy.gov/covid-19-information/
+</t>
+  </si>
+  <si>
+    <t>BIH - Bosnia and Herzegovina</t>
+  </si>
+  <si>
+    <t>Zongyue Liu</t>
+  </si>
+  <si>
+    <t>zongyue.liu@wolfson.ox.ac.uk</t>
+  </si>
+  <si>
+    <t>The government webpage for covid has been regularly updated.
+https://web.archive.org/web/20210401120659/https://www.gouv.bj/coronavirus/
+The government also launched a national vaccination campaign at the end of March 2021.
+https://web.archive.org/web/20210401120207/https://www.gouv.bj/actualite/1228/</t>
+  </si>
+  <si>
+    <t>BEN - Benin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is coded as 1 because in most states, venues for public indoor/outdoor events are open with a specified percentage of original capacity and participants must be adhere to safety measures e.g. It is coded as T because in states like Iowa, mass gatherings and events have no limits on size.
+https://web.archive.org/web/20210403083131/https://www.aarp.org/politics-society/government-elections/info-2020/coronavirus-state-restrictions.html 
+It is important however to note that in some states that use the color-coded framework (risk levels) like Kentucky, counties in the red zone (high risk) are not permitted to have events. 
+Kentucky Red zone - https://web.archive.org/web/20210322120730/https://chfs.ky.gov/agencies/dph/covid19/RedCountyRecommendation.pdf 
+https://web.archive.org/web/20210403082136/https://govstatus.egov.com/kycovid19 
+In Wisconsin, DHS advises (but not mandatory) against attending and hosting gatherings – https://web.archive.org/web/20210403090056/https://www.dhs.wisconsin.gov/covid-19/community.htm
+</t>
+  </si>
+  <si>
+    <t>USA - United States</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Until April 11, essential travel out of the capital area of Ulaanbaatar is restricted with limited exceptions like medical emergencies, funerals, food and gas transport. "There are currently no restrictions on travel into Ulaanbaatar. If traveling from provinces with no infections registered, travelers may enter upon completion of a health questionnaire. However, if traveling from infected areas, entry will be conditioned upon a negative COVID-19 test received within the past 72 hours." See U.S. Embassy and UK Travel Advice websites:
+https://web.archive.org/web/20210403195539/https://mn.usembassy.gov/covid-19-information/
+https://web.archive.org/web/20210403195126/https://www.gov.uk/foreign-travel-advice/mongolia/coronavirus
+</t>
+  </si>
+  <si>
+    <t>MNG - Mongolia</t>
+  </si>
+  <si>
+    <t>María de los Ángeles Lasa</t>
+  </si>
+  <si>
+    <t>ma.angeleslasa@gmail.com</t>
+  </si>
+  <si>
+    <t>"Kosovo’s Ministry of Health has recommended interrupting coronavirus contact tracing. As COVID-19 infected cases grow within the country and restrictive measures are lifted, casting a wide net via contact tracing has put a strain on Kosovo’s testing capabilities, the Ministry claims."
+Source: https://web.archive.org/web/20210404192853/https://exit.al/en/2020/06/22/kosovos-health-ministry-recommends-halting-contact-tracing/
+Note: the article suggests that Kosovo was previously conducting contact tracing, but I couldn't find evidence to support it. If a contact tracing protocol was developed and implemented, that happened likely around March 23, 2020. Source: https://web.archive.org/web/20210404193722/https://www2.deloitte.com/content/dam/Deloitte/al/Documents/legal/Deloitte%20Kosova_Newsletter_COVID-19_6.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RKS - Kosovo </t>
+  </si>
+  <si>
+    <t>Elena Terenzi</t>
+  </si>
+  <si>
+    <t>eterenzi@microsoft.com</t>
+  </si>
+  <si>
+    <t>The maximum number of people visiting a residence is four (4) persons, irrespective of age.
+https://web.archive.org/web/20210405094958/https://www.pio.gov.cy/coronavirus/uploads/22032021_compliancewithmeasuresEN.pdf</t>
+  </si>
+  <si>
+    <t>CYP- Cyprus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nasra Habane </t>
+  </si>
+  <si>
+    <t>nasrahabane@hotmail.co.uk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On the 4th April, the Palestinian authority extended the state of emergency in the West Bank until May 3rd 2021. Wearing a facemask in public continues to be mandatory. Individuals are required to social distance and those who do not follow these guidelines could face possible fines. 
+https://web.archive.org/web/20210405110412/https://www.garda.com/crisis24/news-alerts/463231/palestinian-territories-authorities-extend-state-of-emergency-across-the-west-bank-through-at-least-may-3-update-52 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is no debt and contract relief for households in the Kyrgyz Republic. On December 10, 2020, the Ministry for Social Protection stated that the government has a limited budget for social pension and other social benefits. Accordingly, the government has not announced any new measures that support households during the COVID-19. Moreover, there is no information on debt and contract relief for households on the IMF website. 
+Links: https://archive.vn/qMLrB https://archive.vn/C8sjc https://archive.vn/papLi
+</t>
+  </si>
+  <si>
+    <t>Weekly congregational prayer services in mosques on Fridays and churches on Sundays have been suspended until further notice.
+https://web.archive.org/web/20210329164728/https://www.gov.uk/foreign-travel-advice/jordan/coronavirus</t>
+  </si>
+  <si>
+    <t>JOR - Jordan</t>
+  </si>
+  <si>
+    <t>In HK, ‘a person must wear a mask at all times when the person is boarding or onboard a public transport carrier, is entering or present in an MTR paid area, or is entering or present in a specified public place. … “Public place” means any place to which for the time being the public or a section of the public may or are permitted to have access, whether on payment or otherwise. … it is a reasonable excuse for a person not to wear a mask if the person is engaged in any physical activity (including exercise) that may reasonably be regarded as strenuous for him or her, in a place that is not indoor. … A person who contravenes the requirement of not wearing mask at public place commits an offence and is liable on conviction to a fine at level 3 ($10,000), or may discharge liability for the offence by paying a fixed penalty of $5,000. … The Regulation requires that all person over the age of two must wear mask at all times when the person is boarding or on board a public transport carrier; or entering or present in an MTR paid area. The Regulation applies to the drivers as well (except for public transport that is not in service).’
+https://archive.vn/m6mh3</t>
+  </si>
+  <si>
+    <t>HKG - Hong Kong</t>
+  </si>
+  <si>
+    <t>Fiona Ching Ming Hsu</t>
+  </si>
+  <si>
+    <t>ching.hsu.19@ucl.ac.uk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 April is the first day of resumption of secondary school after 1 year of class suspension while other levels of school has resumed since March.
+https://archive.ph/yoPKm
+https://archive.ph/jDkjV
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MYS - Malaysia </t>
+  </si>
+  <si>
+    <t>Citizens are required to observe social distancing protocols, wear cloth face coverings in public, stay home if they are sick, and seek medical attention if they show symptoms of COVID-19. If you have a fever and/or cough, call 117.
+https://web.archive.org/web/*/https://sl.usembassy.gov/covid-19-information/</t>
+  </si>
+  <si>
+    <t>Per the US Embassy in Yangon, last updated April 7, 2021, gatherings of five or more people are banned.
+Is a curfew in place? – YES
+The military regime has instituted a ban on gatherings of five or more people, and a nationwide curfew from 8:00 P.M. until 4:00 A.M. that supersedes previous COVID-19 policies.
+Are there restrictions on intercity or interstate travel? – YES
+See the US Embassy in Yangon's website, archived at https://archive.vn/WrNQ5.</t>
+  </si>
+  <si>
+    <t>MMR - Myanmar</t>
+  </si>
+  <si>
+    <t>Current interstate restrictions are in place. Several Austrian provinces require a negative COVID-test to enter or exit their borders. Exiting the following regions is only permitted with a negative PCR (not older than 72 hours) or antigen test (not older than 48 hours):
+Burgenland;
+Carinthia;
+Lower Austria: Neunkirchen, Wiener Neustadt Stadt, Wiener Neustadt Land, Scheibbs district;
+Upper Austria: Braunau;
+Salzburg;
+Styria;
+Tyrol: North Tyrol and the Kufstein district, Fulpmes in the Stubai Valley;
+Vorarlberg;
+Vienna.
+https://archive.vn/16jMx
+https://web.archive.org/web/20210410000656/https://at.usembassy.gov/covid-19-information/</t>
+  </si>
+  <si>
+    <t>AUT - Austria</t>
+  </si>
+  <si>
+    <t>Michelle Chan</t>
+  </si>
+  <si>
+    <t>michellewlchan@gmail.com</t>
+  </si>
+  <si>
+    <t>Curfew remains in place from 10PM to 4AM. No changes in policy since the announcement of amendments to public health covid-19 general regulations, valid until the end of April. 
+See the amended regulations from the 26th Covid-19 briefing, posted on facebook by the Ministry of Health and Social Services: 
+https://archive.vn/YxsKl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAM - Namibia </t>
+  </si>
+  <si>
+    <t>The Kingdom of Tonga has extended the National COVID-19 Restrictions Directions until 8pm on 10 May 2021. These include a night time curfew from midnight to 5am. Gatherings are restricted to 50 people at indoor venues and 100 people at outdoor venues, except for religious services and education institutions. Tongan authorities are encouraging social distancing and good hand hygiene. Public places are open including places of worship, shops, restaurants, bars and nightclubs. You must abide by the nationwide curfew and remain in your home or accommodation between midnight and 5am.
+https://web.archive.org/web/20210328181417/https://travelbans.org/oceania-australia/tonga/</t>
+  </si>
+  <si>
+    <t>All travellers are required to display a negative PCR Test on arrival and be submitted to another test 5 days after. During this period, the visitor shall be in quarantine at a "preapproved accommodation".
+https://web.archive.org/web/20210412184534/https://issuu.com/visitbarbados/docs/btmi_travel_protocols_final?fr=sY2JmYjI5MjYzNDk
+https://web.archive.org/web/20210412185401/https://gisbarbados.gov.bb/blog/proposed-entry-protocols-for-vaccinated-visitors/</t>
+  </si>
+  <si>
+    <t>Junu Shrestha</t>
+  </si>
+  <si>
+    <t>shresthajunoo@gmail.com</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/20210401110925/https://www.dabangasudan.org/en/all-news/article/schools-closed-in-sudan-s-red-sea-state-amidst-3rd-covid-19-wave
+No policies were found for stay at home requirement.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDN - Sudan </t>
+  </si>
+  <si>
+    <t>"Some cultural, recreational, sporting, leisure and entertainment facilities have reopened but are subject to limited capacity due to social distancing. Most nightclubs, dance halls, event venues and facilities, sporting academies and gymnastics and martial arts clubs remain closed.
+Until further notice, additional restrictions are in force on the island of São Vincente. Including:
+bars and open air cafés selling alcohol close at 9pm
+restaurants and snack bars close at 9pm"
+https://web.archive.org/web/20210415153339/https://www.gov.uk/foreign-travel-advice/cape-verde/coronavirus</t>
+  </si>
+  <si>
+    <t>CPV - Cape Verde</t>
+  </si>
+  <si>
+    <t>The government provides various information about Covid-19, including advice for the public and statistics.
+https://web.archive.org/web/20210415205401/https://www.coronavirus2020.kz/ru
+https://web.archive.org/web/20210415205639/https://www.gov.kz/memleket/entities/dsm/activities/6625?lang=en</t>
+  </si>
+  <si>
+    <t>Jessica Barreto</t>
+  </si>
+  <si>
+    <t>During research many photo's show leaders and government officials using masks in public, mask wearing is manditory in public as well.  
+----------
+https://web.archive.org/web/20210417161104/https://ci.usembassy.gov/covid-19-information/
+https://web.archive.org/web/20210122002936/https://www.smartraveller.gov.au/destinations/africa/cote-divoire-ivory-coast
+https://web.archive.org/web/20210411181738/https://www.gov.uk/foreign-travel-advice/cote-d-ivoire/coronavirus</t>
+  </si>
+  <si>
+    <t>CIV - Cote d'Ivoire</t>
+  </si>
+  <si>
+    <t>It is not allowed to organize and hold gatherings and celebrations of a private nature (weddings, baptisms, funerals, etc.) with the presence of more than 15 people.
+https://web.archive.org/web/20210419093332/https://coronavirus.bg/bg/910</t>
+  </si>
+  <si>
+    <t>Public places and services
+Markets have reopened as normal.
+Restaurants with a terrace have reopened. A valid negative COVID-19 tests is compulsory for access to a restaurant. Cost of tests are 5000 CFA or approximately £7.00.
+Gatherings of more than 30 people are banned, however, parliament and educational institutions are exempt from this limit.
+All place of worship can only open one day a week. Places of worship with a maximum of 30 people have to observe the ‘sanitary protocol’ which includes compulsory wearing of masks, hand sanitisation, and social distancing.
+Schools will close at 3pm each day to comply with general curfew. Hospital visits are forbidden without authorisation from medical authorities.
+Bars, beaches remain closed.
+Access to restaurants and places of worship is subject to presentation of negative PCR test.
+Wearing of masks in public is compulsory from the age of 5 years old.
+Source: http://web.archive.org/web/20210405145040/https://www.gov.uk/foreign-travel-advice/gabon/coronavirus</t>
+  </si>
+  <si>
+    <t>Adil Sayeed</t>
+  </si>
+  <si>
+    <t>adil.sayeed@utoronto.ca</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/20210420021535/https://www.covid19usvi.com/current-status
+"Safter at home: Current phase -- No gathering greater than 50"</t>
+  </si>
+  <si>
+    <t>Citizens are required to observe social distancing protocols, wear cloth face coverings in public: https://web.archive.org/web/20210420080535/https://sl.usembassy.gov/covid-19-information/ and 
+it is now compulsory to wear a mask when in a vehicle: https://web.archive.org/web/20210420080521/https://www.gov.uk/foreign-travel-advice/sierra-leone/coronavirus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are restrictions between some cities, but “failure to comply” MAY result in penalties 
+“Restrictions have also been introduced on the use of public transport within and between cities. The authorities have stated that failure to comply with these measures may result in penalties including fines or arrest. A reduced flight service still operates between Hargeisa and Addis Ababa for those wishing to leave Somaliland.” 
+http://web.archive.org/web/20210423003742/https://www.smartraveller.gov.au/destinations/africa/somalia </t>
+  </si>
+  <si>
+    <t>Quote (1):
+"All persons must comply with social distancing guidelines of 2 meters (6.5 feet) and wear facemasks while in public. "
+Link (1): http://web.archive.org/web/20210424064306/https://crisis24.garda.com/insights-intelligence/intelligence/risk-alerts/wip10011865826/uzbekistan-health-officials-amend-covid-19-related-entry-requirements-as-of-march-18-update-25
+___________________
+Quote (2):
+"Masks are required in all forms of public transportation and taxis.
+Fines for Non-Compliance: Fines exists for non-compliance of mask-wearing and quarantine violation."
+Link (2): https://web.archive.org/web/20210424064224/https://uz.usembassy.gov/covid-19-information/
+____________________
+Quote (3):
+"You must wear a face mask while outside – you may be fined (up to approximately £100) if you do not comply with this regulation."
+Link (3): http://web.archive.org/web/20210424064257/https://www.gov.uk/foreign-travel-advice/uzbekistan/coronavirus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The government encourages the general public to use the app StaySafe.Ph for digital contact tracing.
+https://web.archive.org/web/*/https://dilg.gov.ph/news/DILG-to-LGUs-public-Use-StaySafePH-app-to-boost-contact-tracing/NC-2021-1062
+</t>
+  </si>
+  <si>
+    <t>PHL - Philippines</t>
+  </si>
+  <si>
+    <t>Cuba has been doing comprehensive contact tracing since the beginning
+“We know scientifically that quick identification of cases, contact tracing and quarantine are the only way to contain the virus in the absence of a vaccine – and because it begins with prevention, the Cuban health system is perfectly suited to carry out that containment strategy.”
+https://web.archive.org/web/20210324150708/https://www.theguardian.com/world/2020/jun/07/cuba-coronavirus-success-contact-tracing-isolation</t>
+  </si>
+  <si>
+    <t>CUB - Cubation 45</t>
+  </si>
+  <si>
+    <t>Cornelia Santoso</t>
+  </si>
+  <si>
+    <t>corneliamelinda@yahoo.com</t>
+  </si>
+  <si>
+    <t>According to the Croatian Institute for Public Health, foreigners with temporary or permanent residency in Croatia can register for the COVID-19 vaccine through their local healthcare provider.  If you have an OIB (Croatian Personal Identification Number) and a local health insurance plan, you may visit https://cijepise.zdravlje.hr/ to register to get vaccinated.  If you do not have a local health insurance plan, you may visit the following Croatian Institute of Public Health website for the contact details of the county public health institutes to register by phone.  Foreigners who are here as tourists cannot register for the vaccine in Croatia.
+http://web.archive.org/web/20210425192137/https://hr.usembassy.gov/covid-19-information-2/</t>
+  </si>
+  <si>
+    <t>Sakina Bano Mendha</t>
+  </si>
+  <si>
+    <t>sakina_356@live.com</t>
+  </si>
+  <si>
+    <t>2 (broad )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As per last updated, the government have provided support in the form of tax reliefs and providing subsidies. 
+Quote: 
+"Key Policy Responses as of March 4, 2021
+To deal with the crisis, Uzbekistan’s government created an Anti-Crisis Fund of US$ 1 billion (about 2 percent of GDP) to fund support to the economy and help those most affected by the crisis. In addition to the Anti-Crisis Fund, the government temporary reduced some taxes and the Fund for Reconstruction and Development increased lending. Specific crisis response measures have included: (i) expanded funding for healthcare, including for medicines, the costs of quarantines, and salary supplements for healthcare works; (ii) an increase in the number of families with children and low-income families receiving social benefits; (iii) assistance to affected businesses via interest subsidies; and (iv) additional public works for infrastructure and to support employment. The authorities also temporary reduced social contributions for individual entrepreneurs, postponed the payment of property and land taxes, extended a moratorium on tax audits, and delayed tax declarations for 2019 income taxes. The central government also asked local governments to reduce taxes by 30 percent and provide a grace period on paying property tax."
+Archived Link
+http://web.archive.org/web/20210425223525/https://www.imf.org/en/Topics/imf-and-covid19/Policy-Responses-to-COVID-19
+</t>
+  </si>
+  <si>
+    <t>4T</t>
+  </si>
+  <si>
+    <t>Ruili is still facing medium level restrictions, the rest of china is at low level restrictions. Medium level restrictions can include quarantining of neighbourhoods and compounds where there are suspected cases.
+Ruili restrictions: 
+https://web.archive.org/web/20210426025738/https://hm.baidu.com/hm.js?64581a73c0c3e650358bb03d7a95eb33
+http://www.vos.com.cn/web/news/gn/content_362661.shtml
+restriction levels:
+https://web.archive.org/web/20210426025818/https://www.garda.com/crisis24/news-alerts/452411/china-authorities-maintaining-international-travel-restrictions-and-domestic-controls-as-of-march-8-update-34</t>
+  </si>
+  <si>
+    <t>CHN - China</t>
+  </si>
+  <si>
+    <t>Mariami Jintcharadze</t>
+  </si>
+  <si>
+    <t>jintcharadze.mariami@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liechtenstein is using SwissCovid app, contact tracing and compliance with the rules as a way to trace people infected with Covid-19. According to the status report in Lichtenstein and Switzerland as of 26 April, 2021 29,861 people who have had contact with infected people are staying in quarantine.  
+https://web.archive.org/web/20210426145506/https://www.covid19.admin.ch/en/overview 
+https://archive.md/bA1qI </t>
+  </si>
+  <si>
+    <t>Aruba received on Wednesday, April 14, 2021, another Pfizer vaccine batch of 30.420 doses.  Aruba has a great number of vaccines available, the Department of Health invites everyone that did not receive their vaccine as yet, to register as soon as practicable for all of us to get vaccinated and be protected.
+http://web.archive.org/web/20210419210502/https://www.government.aw/news/news_47033/item/aruba-receives-another-vaccine-batch_56369.html
+Also, Walk-in vaccination MARATHON drive organized on 24 and 25 April 2021 for all people over 18 who have not yet been vaccinated, at the Teresita Center in San Nicolas, Centro Libertador Betico Croes, Don Bosco Club in Noord or Ritz-Carlton Hotel from 9.00 am pa 4 pm 'NON-STOP'. Please note that the vaccination marathon is only for the first vaccine.
+http://web.archive.org/web/20210427064552/https://www.government.aw/news/news_47033/item/reminder-vaccination-marathon_56410.html</t>
+  </si>
+  <si>
+    <t>ABW - Aruba</t>
   </si>
   <si>
     <t>G96VzPWXk0-0uv5ouFLPkVSWvw_jDgZKm4LZGz53kfBUNUVEUzNPMElMVFcxSUNGNzFDOUZRSUxHQiQlQCN0PWcu</t>
@@ -1929,8 +2271,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:Q137" totalsRowShown="0">
-  <autoFilter ref="A1:Q137" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:Q171" totalsRowShown="0">
+  <autoFilter ref="A1:Q171" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="16"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Start time" dataDxfId="15"/>
@@ -2251,7 +2593,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R137"/>
+  <dimension ref="A1:R171"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
       <selection activeCell="Q4" sqref="Q4"/>
@@ -8231,6 +8573,1468 @@
       </c>
       <c r="P137" s="3"/>
       <c r="Q137" s="3"/>
+    </row>
+    <row r="138" spans="1:17" ht="45">
+      <c r="A138" s="2">
+        <v>139</v>
+      </c>
+      <c r="B138" s="1">
+        <v>44286.555023148147</v>
+      </c>
+      <c r="C138" s="1">
+        <v>44286.562094907407</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E138" s="2"/>
+      <c r="F138" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="G138" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="H138" s="3"/>
+      <c r="I138" s="3"/>
+      <c r="J138" s="4">
+        <v>44286</v>
+      </c>
+      <c r="K138" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L138" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="M138" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N138" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O138" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="P138" s="3"/>
+      <c r="Q138" s="3"/>
+    </row>
+    <row r="139" spans="1:17" ht="75">
+      <c r="A139" s="2">
+        <v>140</v>
+      </c>
+      <c r="B139" s="1">
+        <v>44287.496828703705</v>
+      </c>
+      <c r="C139" s="1">
+        <v>44287.507592592592</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E139" s="2"/>
+      <c r="F139" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="G139" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="H139" s="3"/>
+      <c r="I139" s="3"/>
+      <c r="J139" s="4">
+        <v>44287</v>
+      </c>
+      <c r="K139" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L139" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="M139" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N139" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O139" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="P139" s="3"/>
+      <c r="Q139" s="3"/>
+    </row>
+    <row r="140" spans="1:17" ht="285">
+      <c r="A140" s="2">
+        <v>141</v>
+      </c>
+      <c r="B140" s="1">
+        <v>44289.334282407406</v>
+      </c>
+      <c r="C140" s="1">
+        <v>44289.394652777781</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E140" s="2"/>
+      <c r="F140" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G140" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H140" s="3"/>
+      <c r="I140" s="3"/>
+      <c r="J140" s="4">
+        <v>44287</v>
+      </c>
+      <c r="K140" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="L140" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="M140" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N140" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="O140" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="P140" s="3"/>
+      <c r="Q140" s="3"/>
+    </row>
+    <row r="141" spans="1:17" ht="165">
+      <c r="A141" s="2">
+        <v>142</v>
+      </c>
+      <c r="B141" s="1">
+        <v>44289.782384259262</v>
+      </c>
+      <c r="C141" s="1">
+        <v>44289.839143518519</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E141" s="2"/>
+      <c r="F141" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="G141" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="H141" s="3"/>
+      <c r="I141" s="3"/>
+      <c r="J141" s="4">
+        <v>44289</v>
+      </c>
+      <c r="K141" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="L141" s="8" t="s">
+        <v>469</v>
+      </c>
+      <c r="M141" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N141" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O141" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="P141" s="3"/>
+      <c r="Q141" s="3"/>
+    </row>
+    <row r="142" spans="1:17" ht="165">
+      <c r="A142" s="2">
+        <v>143</v>
+      </c>
+      <c r="B142" s="1">
+        <v>44290.803437499999</v>
+      </c>
+      <c r="C142" s="1">
+        <v>44290.818113425928</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E142" s="2"/>
+      <c r="F142" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="G142" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="H142" s="3"/>
+      <c r="I142" s="3"/>
+      <c r="J142" s="4">
+        <v>44004</v>
+      </c>
+      <c r="K142" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L142" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="M142" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N142" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O142" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="P142" s="3"/>
+      <c r="Q142" s="3"/>
+    </row>
+    <row r="143" spans="1:17" ht="45">
+      <c r="A143" s="2">
+        <v>144</v>
+      </c>
+      <c r="B143" s="1">
+        <v>44291.402800925927</v>
+      </c>
+      <c r="C143" s="1">
+        <v>44291.41028935185</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E143" s="2"/>
+      <c r="F143" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="G143" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="H143" s="3"/>
+      <c r="I143" s="3"/>
+      <c r="J143" s="4">
+        <v>44286</v>
+      </c>
+      <c r="K143" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="L143" s="8" t="s">
+        <v>477</v>
+      </c>
+      <c r="M143" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N143" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O143" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="P143" s="3"/>
+      <c r="Q143" s="3"/>
+    </row>
+    <row r="144" spans="1:17" ht="90">
+      <c r="A144" s="2">
+        <v>145</v>
+      </c>
+      <c r="B144" s="1">
+        <v>44290.554837962962</v>
+      </c>
+      <c r="C144" s="1">
+        <v>44291.467268518521</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E144" s="2"/>
+      <c r="F144" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="G144" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="H144" s="3"/>
+      <c r="I144" s="3"/>
+      <c r="J144" s="4">
+        <v>44290</v>
+      </c>
+      <c r="K144" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="L144" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="M144" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N144" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="O144" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="P144" s="3"/>
+      <c r="Q144" s="3"/>
+    </row>
+    <row r="145" spans="1:17" ht="90">
+      <c r="A145" s="2">
+        <v>146</v>
+      </c>
+      <c r="B145" s="1">
+        <v>44292.389374999999</v>
+      </c>
+      <c r="C145" s="1">
+        <v>44292.394155092596</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E145" s="2"/>
+      <c r="F145" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G145" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="H145" s="3"/>
+      <c r="I145" s="3"/>
+      <c r="J145" s="4">
+        <v>44292</v>
+      </c>
+      <c r="K145" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L145" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="M145" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N145" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="O145" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="P145" s="3"/>
+      <c r="Q145" s="3"/>
+    </row>
+    <row r="146" spans="1:17" ht="45">
+      <c r="A146" s="2">
+        <v>147</v>
+      </c>
+      <c r="B146" s="1">
+        <v>44293.367743055554</v>
+      </c>
+      <c r="C146" s="1">
+        <v>44293.370752314811</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E146" s="2"/>
+      <c r="F146" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G146" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="H146" s="3"/>
+      <c r="I146" s="3"/>
+      <c r="J146" s="4">
+        <v>44293</v>
+      </c>
+      <c r="K146" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L146" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="M146" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N146" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="O146" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="P146" s="3"/>
+      <c r="Q146" s="3"/>
+    </row>
+    <row r="147" spans="1:17" ht="180">
+      <c r="A147" s="2">
+        <v>148</v>
+      </c>
+      <c r="B147" s="1">
+        <v>44293.623472222222</v>
+      </c>
+      <c r="C147" s="1">
+        <v>44293.624837962961</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E147" s="2"/>
+      <c r="F147" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="G147" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="H147" s="3"/>
+      <c r="I147" s="3"/>
+      <c r="J147" s="4">
+        <v>44293</v>
+      </c>
+      <c r="K147" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L147" s="8" t="s">
+        <v>485</v>
+      </c>
+      <c r="M147" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N147" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="O147" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="P147" s="3"/>
+      <c r="Q147" s="3"/>
+    </row>
+    <row r="148" spans="1:17" ht="105">
+      <c r="A148" s="2">
+        <v>149</v>
+      </c>
+      <c r="B148" s="1">
+        <v>44294.538726851853</v>
+      </c>
+      <c r="C148" s="1">
+        <v>44294.548854166664</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E148" s="2"/>
+      <c r="F148" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="G148" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="H148" s="3"/>
+      <c r="I148" s="3"/>
+      <c r="J148" s="4">
+        <v>44291</v>
+      </c>
+      <c r="K148" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L148" s="8" t="s">
+        <v>489</v>
+      </c>
+      <c r="M148" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N148" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O148" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="P148" s="3"/>
+      <c r="Q148" s="3"/>
+    </row>
+    <row r="149" spans="1:17" ht="45">
+      <c r="A149" s="2">
+        <v>150</v>
+      </c>
+      <c r="B149" s="1">
+        <v>44295.788553240738</v>
+      </c>
+      <c r="C149" s="1">
+        <v>44295.843182870369</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E149" s="2"/>
+      <c r="F149" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="G149" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="H149" s="3"/>
+      <c r="I149" s="3"/>
+      <c r="J149" s="4">
+        <v>44295</v>
+      </c>
+      <c r="K149" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L149" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="M149" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N149" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="O149" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="P149" s="3"/>
+      <c r="Q149" s="3"/>
+    </row>
+    <row r="150" spans="1:17" ht="135">
+      <c r="A150" s="2">
+        <v>151</v>
+      </c>
+      <c r="B150" s="1">
+        <v>44296.003831018519</v>
+      </c>
+      <c r="C150" s="1">
+        <v>44296.010462962964</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E150" s="2"/>
+      <c r="F150" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="G150" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="H150" s="3"/>
+      <c r="I150" s="3"/>
+      <c r="J150" s="4">
+        <v>44296</v>
+      </c>
+      <c r="K150" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L150" s="8" t="s">
+        <v>492</v>
+      </c>
+      <c r="M150" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N150" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="O150" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="P150" s="3"/>
+      <c r="Q150" s="3"/>
+    </row>
+    <row r="151" spans="1:17" ht="225">
+      <c r="A151" s="2">
+        <v>152</v>
+      </c>
+      <c r="B151" s="1">
+        <v>44296.003831018519</v>
+      </c>
+      <c r="C151" s="1">
+        <v>44296.014791666668</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E151" s="2"/>
+      <c r="F151" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G151" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H151" s="3"/>
+      <c r="I151" s="3"/>
+      <c r="J151" s="4">
+        <v>44293</v>
+      </c>
+      <c r="K151" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="L151" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="M151" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N151" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O151" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="P151" s="3"/>
+      <c r="Q151" s="3"/>
+    </row>
+    <row r="152" spans="1:17" ht="90">
+      <c r="A152" s="2">
+        <v>153</v>
+      </c>
+      <c r="B152" s="1">
+        <v>44298.419768518521</v>
+      </c>
+      <c r="C152" s="1">
+        <v>44298.42597222222</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E152" s="2"/>
+      <c r="F152" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="G152" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="H152" s="3"/>
+      <c r="I152" s="3"/>
+      <c r="J152" s="4">
+        <v>44298</v>
+      </c>
+      <c r="K152" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L152" s="8" t="s">
+        <v>498</v>
+      </c>
+      <c r="M152" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N152" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="O152" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="P152" s="3"/>
+      <c r="Q152" s="3"/>
+    </row>
+    <row r="153" spans="1:17" ht="120">
+      <c r="A153" s="2">
+        <v>154</v>
+      </c>
+      <c r="B153" s="1">
+        <v>44298.542754629627</v>
+      </c>
+      <c r="C153" s="1">
+        <v>44298.558020833334</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E153" s="2"/>
+      <c r="F153" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G153" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="H153" s="3"/>
+      <c r="I153" s="3"/>
+      <c r="J153" s="4">
+        <v>44298</v>
+      </c>
+      <c r="K153" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L153" s="8" t="s">
+        <v>500</v>
+      </c>
+      <c r="M153" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N153" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="O153" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="P153" s="3"/>
+      <c r="Q153" s="3"/>
+    </row>
+    <row r="154" spans="1:17" ht="90">
+      <c r="A154" s="2">
+        <v>155</v>
+      </c>
+      <c r="B154" s="1">
+        <v>44298.779282407406</v>
+      </c>
+      <c r="C154" s="1">
+        <v>44298.788506944446</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E154" s="2"/>
+      <c r="F154" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="G154" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="H154" s="3"/>
+      <c r="I154" s="3"/>
+      <c r="J154" s="4">
+        <v>44298</v>
+      </c>
+      <c r="K154" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="L154" s="8" t="s">
+        <v>501</v>
+      </c>
+      <c r="M154" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N154" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O154" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="P154" s="3"/>
+      <c r="Q154" s="3"/>
+    </row>
+    <row r="155" spans="1:17" ht="45">
+      <c r="A155" s="2">
+        <v>156</v>
+      </c>
+      <c r="B155" s="1">
+        <v>44299.883819444447</v>
+      </c>
+      <c r="C155" s="1">
+        <v>44299.915335648147</v>
+      </c>
+      <c r="D155" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E155" s="2"/>
+      <c r="F155" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="G155" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="H155" s="3"/>
+      <c r="I155" s="3"/>
+      <c r="J155" s="4">
+        <v>44292</v>
+      </c>
+      <c r="K155" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L155" s="8" t="s">
+        <v>504</v>
+      </c>
+      <c r="M155" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N155" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="O155" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="P155" s="3"/>
+      <c r="Q155" s="3"/>
+    </row>
+    <row r="156" spans="1:17" ht="120">
+      <c r="A156" s="2">
+        <v>157</v>
+      </c>
+      <c r="B156" s="1">
+        <v>44301.633993055555</v>
+      </c>
+      <c r="C156" s="1">
+        <v>44301.654803240737</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E156" s="2"/>
+      <c r="F156" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="G156" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="H156" s="3"/>
+      <c r="I156" s="3"/>
+      <c r="J156" s="4">
+        <v>44298</v>
+      </c>
+      <c r="K156" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="L156" s="8" t="s">
+        <v>506</v>
+      </c>
+      <c r="M156" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N156" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="O156" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="P156" s="3"/>
+      <c r="Q156" s="3"/>
+    </row>
+    <row r="157" spans="1:17" ht="60">
+      <c r="A157" s="2">
+        <v>158</v>
+      </c>
+      <c r="B157" s="1">
+        <v>44301.868321759262</v>
+      </c>
+      <c r="C157" s="1">
+        <v>44301.874039351853</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E157" s="2"/>
+      <c r="F157" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="G157" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="H157" s="3"/>
+      <c r="I157" s="3"/>
+      <c r="J157" s="4">
+        <v>44301</v>
+      </c>
+      <c r="K157" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L157" s="8" t="s">
+        <v>508</v>
+      </c>
+      <c r="M157" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N157" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O157" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="P157" s="3"/>
+      <c r="Q157" s="3"/>
+    </row>
+    <row r="158" spans="1:17" ht="105">
+      <c r="A158" s="2">
+        <v>159</v>
+      </c>
+      <c r="B158" s="1">
+        <v>44304.667326388888</v>
+      </c>
+      <c r="C158" s="1">
+        <v>44304.684652777774</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E158" s="2"/>
+      <c r="F158" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="G158" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="H158" s="3"/>
+      <c r="I158" s="3"/>
+      <c r="J158" s="4">
+        <v>44304</v>
+      </c>
+      <c r="K158" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L158" s="8" t="s">
+        <v>510</v>
+      </c>
+      <c r="M158" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N158" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O158" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="P158" s="3"/>
+      <c r="Q158" s="3"/>
+    </row>
+    <row r="159" spans="1:17" ht="60">
+      <c r="A159" s="2">
+        <v>160</v>
+      </c>
+      <c r="B159" s="1">
+        <v>44305.393043981479</v>
+      </c>
+      <c r="C159" s="1">
+        <v>44305.399571759262</v>
+      </c>
+      <c r="D159" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E159" s="2"/>
+      <c r="F159" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="G159" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="H159" s="3"/>
+      <c r="I159" s="3"/>
+      <c r="J159" s="4">
+        <v>44305</v>
+      </c>
+      <c r="K159" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="L159" s="8" t="s">
+        <v>512</v>
+      </c>
+      <c r="M159" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N159" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O159" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="P159" s="3"/>
+      <c r="Q159" s="3"/>
+    </row>
+    <row r="160" spans="1:17" ht="345">
+      <c r="A160" s="2">
+        <v>161</v>
+      </c>
+      <c r="B160" s="1">
+        <v>44305.832314814812</v>
+      </c>
+      <c r="C160" s="1">
+        <v>44305.835821759261</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E160" s="2"/>
+      <c r="F160" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G160" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="H160" s="3"/>
+      <c r="I160" s="3"/>
+      <c r="J160" s="4">
+        <v>44305</v>
+      </c>
+      <c r="K160" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="L160" s="8" t="s">
+        <v>513</v>
+      </c>
+      <c r="M160" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N160" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="O160" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="P160" s="3"/>
+      <c r="Q160" s="3"/>
+    </row>
+    <row r="161" spans="1:17" ht="30">
+      <c r="A161" s="2">
+        <v>162</v>
+      </c>
+      <c r="B161" s="1">
+        <v>44306.091226851851</v>
+      </c>
+      <c r="C161" s="1">
+        <v>44306.096516203703</v>
+      </c>
+      <c r="D161" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E161" s="2"/>
+      <c r="F161" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="G161" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="H161" s="3"/>
+      <c r="I161" s="3"/>
+      <c r="J161" s="4">
+        <v>44305</v>
+      </c>
+      <c r="K161" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="L161" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="M161" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N161" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O161" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="P161" s="3"/>
+      <c r="Q161" s="3"/>
+    </row>
+    <row r="162" spans="1:17" ht="60">
+      <c r="A162" s="2">
+        <v>163</v>
+      </c>
+      <c r="B162" s="1">
+        <v>44306.326724537037</v>
+      </c>
+      <c r="C162" s="1">
+        <v>44306.339166666665</v>
+      </c>
+      <c r="D162" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E162" s="2"/>
+      <c r="F162" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G162" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H162" s="3"/>
+      <c r="I162" s="3"/>
+      <c r="J162" s="4">
+        <v>44306</v>
+      </c>
+      <c r="K162" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="L162" s="8" t="s">
+        <v>517</v>
+      </c>
+      <c r="M162" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N162" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="O162" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="P162" s="3"/>
+      <c r="Q162" s="3"/>
+    </row>
+    <row r="163" spans="1:17" ht="75">
+      <c r="A163" s="2">
+        <v>164</v>
+      </c>
+      <c r="B163" s="1">
+        <v>44309.029270833336</v>
+      </c>
+      <c r="C163" s="1">
+        <v>44309.030023148145</v>
+      </c>
+      <c r="D163" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E163" s="2"/>
+      <c r="F163" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="G163" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="H163" s="3"/>
+      <c r="I163" s="3"/>
+      <c r="J163" s="4">
+        <v>44308</v>
+      </c>
+      <c r="K163" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="L163" s="8" t="s">
+        <v>518</v>
+      </c>
+      <c r="M163" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N163" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O163" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="P163" s="3"/>
+      <c r="Q163" s="3"/>
+    </row>
+    <row r="164" spans="1:17" ht="409.6">
+      <c r="A164" s="2">
+        <v>165</v>
+      </c>
+      <c r="B164" s="1">
+        <v>44310.269745370373</v>
+      </c>
+      <c r="C164" s="1">
+        <v>44310.282523148147</v>
+      </c>
+      <c r="D164" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E164" s="2"/>
+      <c r="F164" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="G164" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="H164" s="3"/>
+      <c r="I164" s="3"/>
+      <c r="J164" s="4">
+        <v>44310</v>
+      </c>
+      <c r="K164" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="L164" s="8" t="s">
+        <v>519</v>
+      </c>
+      <c r="M164" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N164" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="O164" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="P164" s="3"/>
+      <c r="Q164" s="3"/>
+    </row>
+    <row r="165" spans="1:17" ht="75">
+      <c r="A165" s="2">
+        <v>166</v>
+      </c>
+      <c r="B165" s="1">
+        <v>44311.671018518522</v>
+      </c>
+      <c r="C165" s="1">
+        <v>44311.678310185183</v>
+      </c>
+      <c r="D165" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E165" s="2"/>
+      <c r="F165" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="G165" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="H165" s="3"/>
+      <c r="I165" s="3"/>
+      <c r="J165" s="4">
+        <v>44311</v>
+      </c>
+      <c r="K165" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="L165" s="8" t="s">
+        <v>520</v>
+      </c>
+      <c r="M165" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N165" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O165" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="P165" s="3"/>
+      <c r="Q165" s="3"/>
+    </row>
+    <row r="166" spans="1:17" ht="75">
+      <c r="A166" s="2">
+        <v>167</v>
+      </c>
+      <c r="B166" s="1">
+        <v>44311.680671296293</v>
+      </c>
+      <c r="C166" s="1">
+        <v>44311.682245370372</v>
+      </c>
+      <c r="D166" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E166" s="2"/>
+      <c r="F166" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="G166" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="H166" s="3"/>
+      <c r="I166" s="3"/>
+      <c r="J166" s="4">
+        <v>44311</v>
+      </c>
+      <c r="K166" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="L166" s="8" t="s">
+        <v>522</v>
+      </c>
+      <c r="M166" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N166" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O166" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="P166" s="3"/>
+      <c r="Q166" s="3"/>
+    </row>
+    <row r="167" spans="1:17" ht="120">
+      <c r="A167" s="2">
+        <v>168</v>
+      </c>
+      <c r="B167" s="1">
+        <v>44311.801423611112</v>
+      </c>
+      <c r="C167" s="1">
+        <v>44311.807650462964</v>
+      </c>
+      <c r="D167" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E167" s="2"/>
+      <c r="F167" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="G167" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="H167" s="3"/>
+      <c r="I167" s="3"/>
+      <c r="J167" s="4">
+        <v>44311</v>
+      </c>
+      <c r="K167" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="L167" s="8" t="s">
+        <v>526</v>
+      </c>
+      <c r="M167" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N167" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O167" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="P167" s="3"/>
+      <c r="Q167" s="3"/>
+    </row>
+    <row r="168" spans="1:17" ht="285">
+      <c r="A168" s="2">
+        <v>169</v>
+      </c>
+      <c r="B168" s="1">
+        <v>44311.93959490741</v>
+      </c>
+      <c r="C168" s="1">
+        <v>44311.944837962961</v>
+      </c>
+      <c r="D168" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E168" s="2"/>
+      <c r="F168" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="G168" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="H168" s="3"/>
+      <c r="I168" s="3"/>
+      <c r="J168" s="4">
+        <v>44311</v>
+      </c>
+      <c r="K168" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="L168" s="8" t="s">
+        <v>530</v>
+      </c>
+      <c r="M168" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N168" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="O168" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="P168" s="3"/>
+      <c r="Q168" s="3"/>
+    </row>
+    <row r="169" spans="1:17" ht="165">
+      <c r="A169" s="2">
+        <v>170</v>
+      </c>
+      <c r="B169" s="1">
+        <v>44312.083043981482</v>
+      </c>
+      <c r="C169" s="1">
+        <v>44312.125567129631</v>
+      </c>
+      <c r="D169" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E169" s="2"/>
+      <c r="F169" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G169" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H169" s="3"/>
+      <c r="I169" s="3"/>
+      <c r="J169" s="4">
+        <v>44312</v>
+      </c>
+      <c r="K169" s="7" t="s">
+        <v>531</v>
+      </c>
+      <c r="L169" s="8" t="s">
+        <v>532</v>
+      </c>
+      <c r="M169" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N169" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O169" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="P169" s="3"/>
+      <c r="Q169" s="3"/>
+    </row>
+    <row r="170" spans="1:17" ht="90">
+      <c r="A170" s="2">
+        <v>171</v>
+      </c>
+      <c r="B170" s="1">
+        <v>44312.62736111111</v>
+      </c>
+      <c r="C170" s="1">
+        <v>44312.638981481483</v>
+      </c>
+      <c r="D170" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E170" s="2"/>
+      <c r="F170" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="G170" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="H170" s="3"/>
+      <c r="I170" s="3"/>
+      <c r="J170" s="4">
+        <v>44312</v>
+      </c>
+      <c r="K170" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L170" s="8" t="s">
+        <v>536</v>
+      </c>
+      <c r="M170" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N170" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O170" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="P170" s="3"/>
+      <c r="Q170" s="3"/>
+    </row>
+    <row r="171" spans="1:17" ht="150">
+      <c r="A171" s="2">
+        <v>172</v>
+      </c>
+      <c r="B171" s="1">
+        <v>44313.274525462963</v>
+      </c>
+      <c r="C171" s="1">
+        <v>44313.282951388886</v>
+      </c>
+      <c r="D171" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E171" s="2"/>
+      <c r="F171" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G171" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H171" s="3"/>
+      <c r="I171" s="3"/>
+      <c r="J171" s="4">
+        <v>44311</v>
+      </c>
+      <c r="K171" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="L171" s="8" t="s">
+        <v>537</v>
+      </c>
+      <c r="M171" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N171" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O171" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="P171" s="3"/>
+      <c r="Q171" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8253,17 +10057,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>459</v>
+        <v>539</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>460</v>
+        <v>540</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>461</v>
+        <v>541</v>
       </c>
     </row>
   </sheetData>

</xml_diff>